<commit_message>
feat[DE]: Add conditional formatting
</commit_message>
<xml_diff>
--- a/DataSetExplorer/Core/DataSetSerializer/Template/Clean_Classes_Analysis_Template.xlsx
+++ b/DataSetExplorer/Core/DataSetSerializer/Template/Clean_Classes_Analysis_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ccadet\platform\DataSetExplorer\Core\DataSetSerializer\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3911185D-1AC5-44F2-94CD-F485F5F5E1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09DA36A-F8E9-46C3-8101-AB5E8D55946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Link</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Metrics</t>
+  </si>
+  <si>
+    <t>Suspicious</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -308,11 +314,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -331,27 +337,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:D3 E2:F2">
+  <conditionalFormatting sqref="A5:D5 E4:F4">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>